<commit_message>
This is roaster updates
</commit_message>
<xml_diff>
--- a/Team roster.xlsx
+++ b/Team roster.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e04ffa08d7b11ec/Documents/GitHub/cmpe202-project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunil\OneDrive\Documents\GitHub\cmpe202-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="1" r:id="rId1"/>
@@ -1019,7 +1019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
@@ -1332,7 +1332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>